<commit_message>
push it push it push it
</commit_message>
<xml_diff>
--- a/resultaten/Resultaten na goede Hillclimber/deliverables/wireLengthResultsPartFive.xlsx
+++ b/resultaten/Resultaten na goede Hillclimber/deliverables/wireLengthResultsPartFive.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebruiker\Documents\GitHub\Advanced-Heuristics\resultaten\Resultaten na goede Hillclimber\deliverables\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="384" yWindow="312" windowWidth="18852" windowHeight="9276"/>
+    <workbookView xWindow="380" yWindow="310" windowWidth="18850" windowHeight="9280"/>
   </bookViews>
   <sheets>
     <sheet name="wireLengthResultsPartFive" sheetId="1" r:id="rId1"/>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -569,14 +574,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -587,7 +595,33 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>Wirecost</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nl-NL" baseline="0"/>
+              <a:t> p</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>arameterization: 3 battery types </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -856,6 +890,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2834-407D-B5BA-5CA5C3559733}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1123,6 +1162,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2834-407D-B5BA-5CA5C3559733}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1388,6 +1432,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2834-407D-B5BA-5CA5C3559733}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1429,7 +1478,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1470,7 +1518,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1484,7 +1531,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1503,20 +1549,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>534126</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104140</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>541747</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Grafiek 2"/>
+        <xdr:cNvPr id="3" name="Grafiek 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1577,7 +1629,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1610,9 +1662,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1645,6 +1714,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -1823,13 +1909,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1849,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.57735026899999997</v>
       </c>
@@ -1875,7 +1961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.41633320000000001</v>
       </c>
@@ -1901,7 +1987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.305505046</v>
       </c>
@@ -1927,7 +2013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.305505046</v>
       </c>
@@ -1953,7 +2039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.41633320000000001</v>
       </c>
@@ -1979,7 +2065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.57735026899999997</v>
       </c>
@@ -2005,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.40414518799999999</v>
       </c>
@@ -2031,7 +2117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.251661148</v>
       </c>
@@ -2057,7 +2143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.20816660000000001</v>
       </c>
@@ -2083,7 +2169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.32145502500000001</v>
       </c>
@@ -2109,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.49328828600000002</v>
       </c>
@@ -2135,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.41633320000000001</v>
       </c>
@@ -2161,7 +2247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.23094010800000001</v>
       </c>
@@ -2187,7 +2273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.115470054</v>
       </c>
@@ -2213,7 +2299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.23094010800000001</v>
       </c>
@@ -2239,7 +2325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.41633320000000001</v>
       </c>
@@ -2265,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.251661148</v>
       </c>
@@ -2291,7 +2377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>5.7735027000000001E-2</v>
       </c>
@@ -2317,7 +2403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.152752523</v>
       </c>
@@ -2343,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.35118845799999998</v>
       </c>
@@ -2369,7 +2455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.305505046</v>
       </c>
@@ -2395,7 +2481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.115470054</v>
       </c>
@@ -2421,7 +2507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.115470054</v>
       </c>
@@ -2447,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.305505046</v>
       </c>
@@ -2473,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.20816660000000001</v>
       </c>
@@ -2499,7 +2585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.152752523</v>
       </c>
@@ -2525,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.28867513500000003</v>
       </c>
@@ -2551,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.305505046</v>
       </c>
@@ -2577,7 +2663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.23094010800000001</v>
       </c>
@@ -2603,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.305505046</v>
       </c>
@@ -2629,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.32145502500000001</v>
       </c>
@@ -2655,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.35118845799999998</v>
       </c>
@@ -2681,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.41633320000000001</v>
       </c>
@@ -2707,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.41633320000000001</v>
       </c>
@@ -2733,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.49328828600000002</v>
       </c>
@@ -2759,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.57735026899999997</v>
       </c>

</xml_diff>